<commit_message>
Adding US & Metric variants
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Freelancing\Sprays_scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C20F47F-5B36-4093-A35C-B8AC01BD12C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFB6D0C-6E8F-4C64-A5B8-AEE85A5DDF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14340" yWindow="1728" windowWidth="16380" windowHeight="15276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -920,7 +920,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -959,7 +959,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -975,7 +975,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2">

</xml_diff>